<commit_message>
implemented download sheet function
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">Slave 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfaijfe;la je;lfjas ;fiej</t>
   </si>
   <si>
     <t xml:space="preserve">Slave 5</t>
@@ -151,7 +154,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -165,6 +168,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -291,10 +298,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -541,7 +548,7 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>1</v>
       </c>
@@ -755,15 +762,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>8888888</v>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>12</v>
@@ -840,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>8888888</v>
@@ -908,6 +915,11 @@
         <v>12</v>
       </c>
       <c r="AH8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="4" t="n">
+        <v>22222</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="34">

</xml_diff>